<commit_message>
chore: edit csv file
</commit_message>
<xml_diff>
--- a/cource_price.xlsx
+++ b/cource_price.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Educational\Project\course-finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BD1A7D-CB97-4E51-86AC-925B806E948C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9065B957-BEC5-4DE2-A142-15187D140ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6AEDBDA1-1AC1-458C-A603-276782077778}"/>
   </bookViews>
@@ -36,32 +36,25 @@
     <t>course_price</t>
   </si>
   <si>
-    <t>BSc (Hons) in Information Technology
-Specialising in Software Engineering</t>
+    <t>BSc (Hons) in Information Technology Specialising in Information Systems Engineering</t>
   </si>
   <si>
-    <t>BSc (Hons) in Information Technology
-Specialising in Information Technology</t>
+    <t>BSc (Hons) in Information Technology Specialising in Software Engineering</t>
   </si>
   <si>
-    <t>BSc (Hons) in Information Technology
-Specialising in Computer Systems &amp; Network Engineering</t>
+    <t>BSc (Hons) in Information Technology Specialising in Information Technology</t>
   </si>
   <si>
-    <t>BSc (Hons) in Information Technology
-Specialising in Information Systems Engineering</t>
+    <t>BSc (Hons) in Information Technology Specialising in Computer Systems &amp; Network Engineering</t>
   </si>
   <si>
-    <t>BSc (Hons) in Information Technology
-Specialising in Data Science</t>
+    <t>BSc (Hons) in Information TechnologySpecialising in Data Science</t>
   </si>
   <si>
-    <t>BSc (Hons) in Information Technology
-Specialising in Interactive Media</t>
+    <t>BSc (Hons) in Information Technology Specialising in Interactive Media</t>
   </si>
   <si>
-    <t>BSc (Hons) in Information Technology
-Specialising in Cyber Security</t>
+    <t>BSc (Hons) in Information Technology Specialising in Cyber Security</t>
   </si>
 </sst>
 </file>
@@ -429,7 +422,7 @@
   <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +445,7 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>2013</v>
@@ -463,7 +456,7 @@
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>2014</v>
@@ -474,7 +467,7 @@
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>2015</v>
@@ -485,7 +478,7 @@
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>2016</v>
@@ -496,7 +489,7 @@
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>2017</v>
@@ -507,7 +500,7 @@
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>2018</v>
@@ -518,7 +511,7 @@
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>2019</v>
@@ -529,7 +522,7 @@
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>2020</v>
@@ -540,7 +533,7 @@
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>2021</v>
@@ -551,7 +544,7 @@
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>2022</v>
@@ -562,7 +555,7 @@
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>2023</v>
@@ -573,7 +566,7 @@
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>2013</v>
@@ -584,7 +577,7 @@
     </row>
     <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>2014</v>
@@ -595,7 +588,7 @@
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>2015</v>
@@ -606,7 +599,7 @@
     </row>
     <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>2016</v>
@@ -617,7 +610,7 @@
     </row>
     <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>2017</v>
@@ -628,7 +621,7 @@
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18">
         <v>2018</v>
@@ -639,7 +632,7 @@
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B19">
         <v>2019</v>
@@ -650,7 +643,7 @@
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B20">
         <v>2020</v>
@@ -661,7 +654,7 @@
     </row>
     <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21">
         <v>2021</v>
@@ -672,7 +665,7 @@
     </row>
     <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22">
         <v>2022</v>
@@ -683,7 +676,7 @@
     </row>
     <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B23">
         <v>2023</v>
@@ -694,7 +687,7 @@
     </row>
     <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B24">
         <v>2013</v>
@@ -705,7 +698,7 @@
     </row>
     <row r="25" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25">
         <v>2014</v>
@@ -716,7 +709,7 @@
     </row>
     <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26">
         <v>2015</v>
@@ -727,7 +720,7 @@
     </row>
     <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B27">
         <v>2016</v>
@@ -738,7 +731,7 @@
     </row>
     <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B28">
         <v>2017</v>
@@ -749,7 +742,7 @@
     </row>
     <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29">
         <v>2018</v>
@@ -760,7 +753,7 @@
     </row>
     <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30">
         <v>2019</v>
@@ -771,7 +764,7 @@
     </row>
     <row r="31" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B31">
         <v>2020</v>
@@ -782,7 +775,7 @@
     </row>
     <row r="32" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B32">
         <v>2021</v>
@@ -793,7 +786,7 @@
     </row>
     <row r="33" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B33">
         <v>2022</v>
@@ -804,7 +797,7 @@
     </row>
     <row r="34" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B34">
         <v>2023</v>
@@ -815,7 +808,7 @@
     </row>
     <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B35">
         <v>2013</v>
@@ -826,7 +819,7 @@
     </row>
     <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B36">
         <v>2014</v>
@@ -837,7 +830,7 @@
     </row>
     <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <v>2015</v>
@@ -848,7 +841,7 @@
     </row>
     <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B38">
         <v>2016</v>
@@ -859,7 +852,7 @@
     </row>
     <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B39">
         <v>2017</v>
@@ -870,7 +863,7 @@
     </row>
     <row r="40" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B40">
         <v>2018</v>
@@ -881,7 +874,7 @@
     </row>
     <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B41">
         <v>2019</v>
@@ -892,7 +885,7 @@
     </row>
     <row r="42" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B42">
         <v>2020</v>
@@ -903,7 +896,7 @@
     </row>
     <row r="43" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B43">
         <v>2021</v>
@@ -914,7 +907,7 @@
     </row>
     <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B44">
         <v>2022</v>
@@ -925,7 +918,7 @@
     </row>
     <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B45">
         <v>2023</v>

</xml_diff>